<commit_message>
added further estimate to tuitionFees
</commit_message>
<xml_diff>
--- a/estimates/tuitionFees.xlsx
+++ b/estimates/tuitionFees.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>estimate</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>uses lasso regression; the paper argues that traditional DiD approaches suffer from high dimensionality issues and cannot identify the true effect</t>
+  </si>
+  <si>
+    <t>Huber (2012), Table 5</t>
+  </si>
+  <si>
+    <t>enrollment_rate_pp_huber_did</t>
+  </si>
+  <si>
+    <t>Huber (2012) argues that this is a lower bound. There is also a model of university enrollment in the paper which suggests that the true value is approximated by 4.7</t>
+  </si>
+  <si>
+    <t>Do tuition fees affect enrollment behavior? Evidence from a ‘natural experiment’ in Germany (repec.org)</t>
   </si>
 </sst>
 </file>
@@ -919,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1029,7 @@
         <v>9.8600000000000007E-3</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>16</v>
@@ -1040,7 +1052,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1050,6 +1062,29 @@
       </c>
       <c r="M4" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>-2.6800000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1057,8 +1092,9 @@
     <hyperlink ref="L3" r:id="rId1"/>
     <hyperlink ref="L2" r:id="rId2"/>
     <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4" display="https://ideas.repec.org/a/eee/ecoedu/v31y2012i6p949-960.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>